<commit_message>
have done OCR on judgements downloaded
</commit_message>
<xml_diff>
--- a/check api/judgments_output.xlsx
+++ b/check api/judgments_output.xlsx
@@ -453,17 +453,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>**Crime Scenario:*** On January 3, 2015, Muhammad Mustafa, a 18-19 year old plumber, went out of his house on his motorcycle to Liaquat Bazar, Quetta.* He had two mobile phone SIM numbers, 0311-1842119 and 0313-2280082.* When his brother, Muhammad Hassan, could not contact him, he contacted their friend, Abdul Latif, who told him that Mustafa had given him another SIM number.* On January 8, 2015, Muhammad Hassan saw a publication in a newspaper that led him to the mortuary, where he found his brother's dead body with a strangulation mark on the neck and the right eye removed.* The police registered a case against unknown accused, and later implicated Rehmatullah, Naseer Ahmad, and Muhammad Younas in the case based on circumstantial evidence.</t>
+          <t>**Crime Scenario:*** The appellants, Rehmatullah, Naseer Ahmad, and Muhammad Younas, were tried for the murder of Muhammad Mustafa, a 18-19 year old plumber, who was found dead with a strangulation mark on his neck and his right eye removed.* The FIR was registered on January 3, 2015, and the investigation led to the appellants being implicated in the case.* The prosecution's case was based on alleged confessions, recovery of a mobile phone and motorcycle, and pointing out of the place of occurrence and recovery of the dead body.* The appellants denied the allegations and claimed innocence.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>**Witnesses:*** Muhammad Hassan, the complainant and brother of the deceased, did not enter appearance in the witness box.* Mansoor Ahmed, SI (PW-2), and Naseebullah, ASI (PW-3), testified about the alleged extra judicial confession of Muhammad Younas, appellant.* Dr. Ali Mardan, (PW-7), testified about the medical evidence, including the removal of the right eye of the deceased.</t>
+          <t>**Witnesses:*** 07 witnesses were produced by the prosecution, including Mansoor Ahmed, SI (PW-2), Naseebullah, ASI (PW-3), Abdul Rahim Khokhar, I.P. (PW-6), and Dr. Ali Mardan (PW-7).* The appellants did not make any statements on oath and did not produce any evidence in their defense.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>**Judgment:*** The appellants, Rehmatullah, Naseer Ahmad, and Muhammad Younas, were convicted of murder under Section 302(b) PPC read with Section 34 PPC and sentenced to imprisonment for life.* The High Court upheld the judgment of the learned Trial Court.* The Supreme Court allowed the appeals and acquitted the appellants, stating that the circumstantial evidence produced in the case was not worthy of reliance and the prosecution had failed to prove its case beyond a reasonable doubt.* The court held that the prosecution's case was replete with contradictions and inconsistencies, and that the alleged extra judicial confession of Muhammad Younas was unreliable and inadmissible in evidence.* The court also noted that the medical evidence did not support the prosecution's case, and that the alleged motive of sodomy was not proved.* The appellants were ordered to be released from jail forthwith unless required to be detained in any other case.</t>
+          <t>**Judgment:*** The Supreme Court allowed the appeals and acquitted the appellants of the charges.* The court held that the circumstantial evidence produced by the prosecution was not worthy of reliance and failed to prove the case against the appellants beyond a reasonable doubt.* The court noted that the prosecution's case was based on alleged confessions, which were inadmissible in evidence, and that the recovery of the mobile phone and motorcycle was not properly established.* The court also noted that the pointing out of the place of occurrence and recovery of the dead body was not reliable evidence.* The court concluded that the prosecution had miserably failed to prove its case against the appellants and that the appellants were entitled to an acquittal.**Basis of Decision:*** The court applied the principles of circumstantial evidence, holding that every circumstance should be linked to each other and form a continuous chain that touches the dead body and the accused.* The court also applied the principle that the confession of an accused before the police while in custody is inadmissible in evidence.**Section of Law Applied:*** The court applied the Pakistan Penal Code (PPC) and the Code of Criminal Procedure (CrPC).</t>
         </is>
       </c>
     </row>

</xml_diff>